<commit_message>
🔥_chore(frontend): removing and updating code
</commit_message>
<xml_diff>
--- a/demos/CPCTestSample.xlsx
+++ b/demos/CPCTestSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkit/FullStack_local/myApps/uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkit/FullStack_local/myApps/examiner-portfolio/demos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F103114B-BFD4-3342-82E3-B61DAFF86039}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807C2158-D3E6-3143-B31B-CF3BFD2726C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1560" windowWidth="16380" windowHeight="17600" xr2:uid="{0A05F397-D17A-A848-93DB-B27094F29A32}"/>
   </bookViews>
@@ -84,10 +84,10 @@
     <t>B29L2031/06</t>
   </si>
   <si>
-    <t>B29C7044</t>
-  </si>
-  <si>
     <t>A22C13/0013</t>
+  </si>
+  <si>
+    <t>B29C70/44</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,7 +862,7 @@
     <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>8</v>
@@ -886,7 +886,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>8</v>

</xml_diff>